<commit_message>
Update 909 - UK Omicron reported cases.xlsx
</commit_message>
<xml_diff>
--- a/909 - UK Omicron reported cases.xlsx
+++ b/909 - UK Omicron reported cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hp-server\ServerFolders\Documents\Covid-19\Covid data\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BE9F22-5D75-4011-961E-D1ABE1D1CF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C334E0A-082C-46AA-A3F0-C51CA07DBE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="240" windowWidth="26415" windowHeight="20910" activeTab="1" xr2:uid="{3C40590B-D4B6-470C-B0F2-DCBF10F87F6E}"/>
+    <workbookView xWindow="60" yWindow="240" windowWidth="27870" windowHeight="20910" activeTab="1" xr2:uid="{3C40590B-D4B6-470C-B0F2-DCBF10F87F6E}"/>
   </bookViews>
   <sheets>
     <sheet name="&lt; dec 3" sheetId="1" r:id="rId1"/>
@@ -371,10 +371,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Daily!$A$2:$A$11</c:f>
+              <c:f>Daily!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -404,6 +404,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -417,10 +420,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Daily!$B$2:$B$11</c:f>
+              <c:f>Daily!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -450,6 +453,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -493,10 +499,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Daily!$A$2:$A$11</c:f>
+              <c:f>Daily!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -526,6 +532,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -539,10 +548,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Daily!$C$2:$C$11</c:f>
+              <c:f>Daily!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
@@ -566,6 +575,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -609,10 +621,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Daily!$A$2:$A$11</c:f>
+              <c:f>Daily!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -642,6 +654,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -655,15 +670,18 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Daily!$D$2:$D$11</c:f>
+              <c:f>Daily!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -727,13 +745,13 @@
                           <c15:sqref>Daily!$A$2:$A$20</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Daily!$A$2:$A$11</c15:sqref>
+                          <c15:sqref>Daily!$A$2:$A$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>d/m</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>44527</c:v>
                       </c:pt>
@@ -763,6 +781,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>44536</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44537</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -775,13 +796,13 @@
                           <c15:sqref>Daily!$A$2:$A$17</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Daily!$A$2:$A$11</c15:sqref>
+                          <c15:sqref>Daily!$A$2:$A$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>d/m</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>44527</c:v>
                       </c:pt>
@@ -811,6 +832,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>44536</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44537</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -861,13 +885,13 @@
                           <c15:sqref>Daily!$A$2:$A$20</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Daily!$A$2:$A$11</c15:sqref>
+                          <c15:sqref>Daily!$A$2:$A$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>d/m</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>44527</c:v>
                       </c:pt>
@@ -897,6 +921,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>44536</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44537</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -909,13 +936,13 @@
                           <c15:sqref>Daily!$E$2:$E$20</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Daily!$E$2:$E$11</c15:sqref>
+                          <c15:sqref>Daily!$E$2:$E$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -932,6 +959,139 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Daily!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UK daily</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>27/11</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>28/11</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>29/11</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>30/11</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1/12</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>2/12</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>3/12</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>4/12</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>5/12</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>6/12</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>7/12</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>7/12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>7/12</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>7/12</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Daily!$F$2:$F$17</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Daily!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-39C3-4DF6-8BA7-B9B3A66A9FD9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -944,99 +1104,7 @@
         <c:smooth val="0"/>
         <c:axId val="611681088"/>
         <c:axId val="611685680"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="5"/>
-                <c:order val="5"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Daily!$F$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>UK daily</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:srgbClr val="00B050"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>Daily!$F$2:$F$17</c15:sqref>
-                        </c15:fullRef>
-                        <c15:formulaRef>
-                          <c15:sqref>Daily!$F$2:$F$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                      <c:pt idx="0">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>92</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>26</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>86</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>90</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-39C3-4DF6-8BA7-B9B3A66A9FD9}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:lineChart>
       <c:dateAx>
         <c:axId val="611681088"/>
@@ -1425,10 +1493,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -1458,6 +1526,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1471,10 +1542,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$B$2:$B$11</c:f>
+              <c:f>Cum!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1504,6 +1575,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1547,10 +1621,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -1580,6 +1654,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1593,10 +1670,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$C$2:$C$11</c:f>
+              <c:f>Cum!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1626,6 +1703,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1669,10 +1749,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -1702,6 +1782,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1715,10 +1798,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$D$2:$D$11</c:f>
+              <c:f>Cum!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1748,6 +1831,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1811,13 +1897,13 @@
                           <c15:sqref>Cum!$A$2:$A$20</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Cum!$A$2:$A$11</c15:sqref>
+                          <c15:sqref>Cum!$A$2:$A$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>d/m</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>44527</c:v>
                       </c:pt>
@@ -1847,6 +1933,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>44536</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44537</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1859,13 +1948,13 @@
                           <c15:sqref>Cum!$E$2:$E$20</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Cum!$E$2:$E$11</c15:sqref>
+                          <c15:sqref>Cum!$E$2:$E$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
                       </c:pt>
@@ -1894,6 +1983,9 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1947,10 +2039,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -1980,6 +2072,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1993,10 +2088,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$F$2:$F$11</c:f>
+              <c:f>Cum!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2026,6 +2121,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2437,10 +2535,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -2470,6 +2568,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2483,10 +2584,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$B$2:$B$11</c:f>
+              <c:f>Cum!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2516,6 +2617,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2559,10 +2663,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -2592,6 +2696,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2605,10 +2712,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$C$2:$C$11</c:f>
+              <c:f>Cum!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2638,6 +2745,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2681,10 +2791,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -2714,6 +2824,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2727,10 +2840,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$D$2:$D$11</c:f>
+              <c:f>Cum!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2760,6 +2873,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2823,13 +2939,13 @@
                           <c15:sqref>Cum!$A$2:$A$20</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Cum!$A$2:$A$11</c15:sqref>
+                          <c15:sqref>Cum!$A$2:$A$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>d/m</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>44527</c:v>
                       </c:pt>
@@ -2859,6 +2975,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>44536</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44537</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2871,13 +2990,13 @@
                           <c15:sqref>Cum!$E$2:$E$20</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Cum!$E$2:$E$11</c15:sqref>
+                          <c15:sqref>Cum!$E$2:$E$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
                       </c:pt>
@@ -2906,6 +3025,9 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
                         <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
@@ -2959,10 +3081,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$A$2:$A$11</c:f>
+              <c:f>Cum!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>d/m</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44527</c:v>
                 </c:pt>
@@ -2992,6 +3114,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3005,10 +3130,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Cum!$F$2:$F$11</c:f>
+              <c:f>Cum!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -3038,6 +3163,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6639,10 +6767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02A7B23-D2B9-478B-A8F1-4D081290DAD3}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6824,6 +6952,24 @@
         <v>90</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>44537</v>
+      </c>
+      <c r="B12">
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f>SUM(B12:E12)</f>
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6833,10 +6979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0BE4646-BADC-4720-B827-74C8D9493DDA}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V35" sqref="U35:V35"/>
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7115,6 +7261,31 @@
         <v>336</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>44537</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B11+Daily!B12)</f>
+        <v>333</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C11+Daily!C12)</f>
+        <v>99</v>
+      </c>
+      <c r="D12">
+        <f>SUM(D11+Daily!D12)</f>
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E11+Daily!E12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12" si="1">SUM(B12:D12)</f>
+        <v>437</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>